<commit_message>
Add h30-h35 for fatigue enhanced data
</commit_message>
<xml_diff>
--- a/SubjectsInfo.xlsx
+++ b/SubjectsInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeNicData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeNicData\SeNic\SeNic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B36034-5151-49D7-99A3-D50D270D104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD3893D-7624-40E7-AABD-DA3E4937C205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15330" yWindow="-5400" windowWidth="13725" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t>h0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +191,33 @@
   <si>
     <t>Sessions</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h30</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>h31</t>
+  </si>
+  <si>
+    <t>h32</t>
+  </si>
+  <si>
+    <t>h33</t>
+  </si>
+  <si>
+    <t>h34</t>
+  </si>
+  <si>
+    <t>h35</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -213,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -293,6 +326,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1585,6 +1621,198 @@
         <v>44</v>
       </c>
     </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="3">
+        <v>23</v>
+      </c>
+      <c r="D32" s="3">
+        <v>54</v>
+      </c>
+      <c r="E32" s="3">
+        <v>166</v>
+      </c>
+      <c r="F32" s="3">
+        <v>24.9</v>
+      </c>
+      <c r="G32" s="3">
+        <v>24.1</v>
+      </c>
+      <c r="H32" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="3">
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>62</v>
+      </c>
+      <c r="E33" s="3">
+        <v>172</v>
+      </c>
+      <c r="F33" s="3">
+        <v>26.2</v>
+      </c>
+      <c r="G33" s="3">
+        <v>25.6</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="I33" s="8">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="3">
+        <v>27</v>
+      </c>
+      <c r="D34" s="3">
+        <v>58</v>
+      </c>
+      <c r="E34" s="3">
+        <v>169</v>
+      </c>
+      <c r="F34" s="3">
+        <v>25.4</v>
+      </c>
+      <c r="G34" s="3">
+        <v>24.3</v>
+      </c>
+      <c r="H34" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I34" s="8">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="3">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3">
+        <v>72</v>
+      </c>
+      <c r="E35" s="3">
+        <v>179</v>
+      </c>
+      <c r="F35" s="3">
+        <v>25.8</v>
+      </c>
+      <c r="G35" s="3">
+        <v>26</v>
+      </c>
+      <c r="H35" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="I35" s="8">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="3">
+        <v>28</v>
+      </c>
+      <c r="D36" s="3">
+        <v>75</v>
+      </c>
+      <c r="E36" s="3">
+        <v>174</v>
+      </c>
+      <c r="F36" s="3">
+        <v>25.6</v>
+      </c>
+      <c r="G36" s="3">
+        <v>26.8</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="I36" s="8">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="3">
+        <v>25</v>
+      </c>
+      <c r="D37" s="3">
+        <v>46</v>
+      </c>
+      <c r="E37" s="3">
+        <v>159</v>
+      </c>
+      <c r="F37" s="3">
+        <v>23.8</v>
+      </c>
+      <c r="G37" s="3">
+        <v>20.7</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>